<commit_message>
adicionando dados à planilha dos algoritmos
</commit_message>
<xml_diff>
--- a/Algoritmos.xlsx
+++ b/Algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guich\Documents\PDPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18B3E65-0399-437C-9744-F6416DAB3A51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E15C5C2-901A-4E3C-AC4D-C241C5FA57B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -42,15 +42,94 @@
     <t>Maxent</t>
   </si>
   <si>
-    <t>Não necessita de dados de ausência, o que ajuda com problemas de registros de ausência duvidosos</t>
+    <t>Não necessita de dados de ausência, o que ajuda com problemas de registros de ausência duvidosos e falta de dados</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; Apenas com dados de ocorrência não é possível determinar exatamente a prevalência da espécie na paisagem (que seria a proporção de locais ocupados). 
+&gt; Outra limitação de usar apenas dados de presença é o viés na seleção dos registros (algumas áreas nas paisagens são mais amostradas do que outras), o que tem um efeito maior em modelos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">presence-only </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">do que em </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>presence-absence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+&gt; (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A statistical explanation of MaxEnt for ecologists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Elith, Jane
+Phillips et al.)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -100,6 +179,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,7 +475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,21 +495,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>

</xml_diff>

<commit_message>
adicionando dados à planilha Algoritmos
</commit_message>
<xml_diff>
--- a/Algoritmos.xlsx
+++ b/Algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guich\Documents\PDPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D369231-F747-426D-94A7-42F3E8870BF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923F76D-3712-41CC-ADD3-D195F71424BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00FA97CC-6BB4-410B-81B2-38C9B716A4ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>GARP (Genetic Algorithm for Rule Set Production)</t>
   </si>
@@ -60,11 +60,6 @@
 &gt; Combinação de diversos métodos matemáticos e estatísticos, o uso de cada método vai depender da quantidade de dados de ocorrências e variáveis ambientais e dos tipos de dados.</t>
   </si>
   <si>
-    <t>&gt; Apenas com dados de ocorrência não é possível determinar exatamente a prevalência da espécie na paisagem (que seria a proporção de locais ocupados). 
-&gt; Outra limitação de usar apenas dados de presença é o viés na seleção dos registros (algumas áreas nas paisagens são mais amostradas do que outras), o que tem um efeito maior em modelos presence-only do que em presence-absence.
-&gt; (A statistical explanation of MaxEnt for ecologists - Elith, Jane Phillips et al.)</t>
-  </si>
-  <si>
     <t>&gt; Machine learning
 Maxent é um algoritmo de machine learning, que através do input das camadas ambientais e dados de presença das espécies cria um modelo que tenta maximizar a distribuição provável da espécie (máxima entropia).
 Retorna três outputs que servem para diferentes interpretações, um output é a logística, que mostra a probabilidade de presenca em cada grid.</t>
@@ -109,6 +104,94 @@
 &gt; Maximum entropy modelling of species geographic distributions (Philips et al. 2006)
 &gt; Philips et al. (2004) em outro estudo anterior também compararam modelos gerados pelo GARP e Maxent de 12 espécies, utilizando-se de métodos estatísticos e quantidades diferentes de dados de treino (ocorrências). Com 10 ocorrências os modelos produzidos pelo Maxent tiveram acurácia ligeiramente melhor e conforme a quantidade de ocorrências para treino aumentaram logaritmicamente(e mais features utilizadas), os indíces de performance do Maxent também aumentaram, perforando melhor que GARP na maioria dos modelos.
 &gt; A Maximum Entropy Approach to Species Distribution Modeling (Philips et al. 2004)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; GARP é o segundo algoritmo de modelagem de distribuição mais usado, estando atrás apenas do Maxent
+&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Painting maps with bats: species distribution modelling in bat research and conservation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Orly Razgour et al. 2016)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Apenas com dados de ocorrência não é possível determinar exatamente a prevalência da espécie na paisagem (que seria a proporção de locais ocupados). 
+&gt; Outra limitação de usar apenas dados de presença é o viés na seleção dos registros (algumas ocorrências nas paisagens são mais amostradas do que outras, como possuem características geográficas semelhantes, isso pode inflar as estimativas), o que tem um efeito maior em modelos presence-only do que em presence-absence.
+&gt; (A statistical explanation of MaxEnt for ecologists - Elith, Jane Phillips et al.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; Pearson et al. (2007) modelaram a distribuição potencial de 13 espécies de largatixas de Madagascar utilizando Maxent e GARP e abordagem estatística </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jackknife</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, foram utilizados de 4 a 23 ocorrências. Com menos de 10 ocorrências, Maxent teve maiores taxas de sucesso do que GARP, enquanto que este ainda sim obteve um desempenho relativamente bom.
+&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Predicting species distributions from small numbers of occurrence records: a test case using cryptic geckos in Madagascar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Richard Peterson et al. 2007)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Wisz et al. (2008) utilizaram 12 algoritmos para a modelagem da distribuição de 46 espécies de 6 diferentes regiões do planeta, 3 tamanhos de amostras (100, 30 e 10 ocorrências) para o treino dos modelos e dados de ausência e presença estratégicos para estimar os modelos. As predições foram avaliadas a partir do AUC do ROC e taxa de correlação. O modelo com melhores indíces e com 10 ocorrências utilizadas foi Maxent, seguido pelo GARP, com uma diferença significativa. Com 30 ocorrências, GBM ( Generalised Boosted Models), Maxent e GARP performaram melhor. Com 100 ocorrências, GBM e Maxent obtiveram os melhores índices AUC.
+&gt; Com a diminuição do tamanho das amostras, a acurácia dos modelos também diminuíram. 
+&gt; Maxent mostrou ter uma performance consistente ao longo de diferentes quantidades de ocorrências de treino, uma explicação dada pelos autores é o uso de regularização pelo Maxexnt, evitando sobreajuste.
+&gt; Os autores também destacaram a performance do Maxent e GARP em criar modelos concisos com poucas ocorrências 
+&gt; Effects of sample size on the performance of species distribution models (Wisz et al. 2008)</t>
   </si>
 </sst>
 </file>
@@ -144,7 +227,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -246,8 +329,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,11 +646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F280F5-24EE-4664-8BA0-7ED3FDBE296D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -596,84 +679,95 @@
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="186" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="290.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" ht="301.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:3" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionando artigos à tabela de algoritmos
</commit_message>
<xml_diff>
--- a/Algoritmos.xlsx
+++ b/Algoritmos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guich\Documents\PDPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923F76D-3712-41CC-ADD3-D195F71424BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1958C1-8ACD-419A-8EDC-8E013304410A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00FA97CC-6BB4-410B-81B2-38C9B716A4ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>GARP (Genetic Algorithm for Rule Set Production)</t>
   </si>
@@ -193,12 +193,365 @@
 &gt; Os autores também destacaram a performance do Maxent e GARP em criar modelos concisos com poucas ocorrências 
 &gt; Effects of sample size on the performance of species distribution models (Wisz et al. 2008)</t>
   </si>
+  <si>
+    <t>Artigo, autores e ano</t>
+  </si>
+  <si>
+    <t>Revista</t>
+  </si>
+  <si>
+    <t>Pontos chave</t>
+  </si>
+  <si>
+    <t>Global Change Biology</t>
+  </si>
+  <si>
+    <t>&gt; Avaliaram a abilidade de 4 modelos de envelope (Bioclim, Domain, GAM e Maxent) em predizer a distribuição de espécies no presente, passado (21000 anos atrás) e futuro (sob ação das mudanças climáticas) ao comparar as predições com as feitas por modelos mecanísticos (MM);</t>
+  </si>
+  <si>
+    <t>&gt; MM são modelos obtidos com base nos conhecimentos sobre a fisiologia da espécie, portanto mais confiável;</t>
+  </si>
+  <si>
+    <t>&gt; Utilizadas 100 espécies de plantas da América do Sul para criar os modelos mecanísticos e os modelos de envelope;</t>
+  </si>
+  <si>
+    <t>&gt; Para avaliar o quão bem os modelos de envelope predizeram em relação ao MM foram usados 4 índices: Tamanho Relativo do Alcance (RRS), Índice de Sobreposição (OI), Taxa de Falso Positivo (FPR) e Taxa de Falso Negativo (FNR)</t>
+  </si>
+  <si>
+    <t>RESULTADOS: &gt; Maxent obteve o maior valor de sobreposição OI, 0.91, utilizando 6 variáveis ambientais. Bioclim obeteve OI de 0.90, GAM 0.84 e Domain 0.77.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The ability of climate envelope to predict the effect of climate change on species distributions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ Robert Hijmans &amp; Catherine Graham (2006)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Os melhores modelos foram preditos por Maxent e GAM
+&gt; Segundo os autores, GAM pode ser mais apropriado caso o objetivo seja predizer a propensão de espécies a serem extintas, devido ao RRS ter sido mais fiel com o MM.</t>
+  </si>
+  <si>
+    <t>&gt; Maxent teve maior concordância com o MM, apresentando alto OI, e baixos valores de valso negativo e positivo, ao custo de leve aumento no RRS</t>
+  </si>
+  <si>
+    <t>&gt; Bioclim foi indicado pelos autores como bom para fins de conservação, pois embora provavelmente tenha subestimado o tamanho dos alcances das espécies, há grandes chances de que áreas adequadas sejam identificadas corretamente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; Domain performou pobremente, subestimando o alcance das espécies para as condições futura e passada. Os autores aconselharam a evitar o Domain para predições sob condições de mudanças climáticas. </t>
+  </si>
+  <si>
+    <t>Ecography</t>
+  </si>
+  <si>
+    <t>&gt; Para avaliar os modelos gerados utilizaram 3 métodos estatísticos: 1) O AUC (Area under the curve) do ROC (Receiver Operating  Curves) 2)o sucesso de predição e 3) A comparação espacial com as predições geradas por modelos com todas as ocorrências da espécie.</t>
+  </si>
+  <si>
+    <t>&gt; Testaram 4 métodos de modelagem (Bioclim, Domain, GARP e Maxent) ao modelar a distribuição de 18 espécies utilizando seis tamanhos de amostragem diferentes (5, 10, 25, 50, 75 e 100 ocorrências de presença) para treino e 50 ocorrências para teste.</t>
+  </si>
+  <si>
+    <t>&gt; Para cada espécie foram gerados 244 modelos: 10 modelos para cada método de modelagem para cada um dos 6 tamanhos de amostra e 1 modelo com 150 ocorrências (o dataset todo)</t>
+  </si>
+  <si>
+    <t>&gt; RESULTADOS: &gt; Os valores de AUC foram no geral altos para as amostras com 100 ocorrências, exceto pra o GARP;
+&gt; O AUC aumentaram com o tamanho das amostras</t>
+  </si>
+  <si>
+    <t>&gt; Nos modelos do Bioclim, AUC alcançou o valor máximo em 75 ocorrências; em 50 para Maxent e Domain; 10 para GARP, que se  manteve consistente ao longo dos tamanhos de amostras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; O sucesso de predição aumentou com o tamanho das amostras. Com tamanhos entre 5 e 25 ocorrências, a maior performance para a menor foi: Maxent, GARP, Domain e Bioclim. </t>
+  </si>
+  <si>
+    <t>&gt; A menor variação nos valores de sucesso de predição de 5 a 100 ocorrências foi pelo Maxent, seguido por GARP</t>
+  </si>
+  <si>
+    <t>&gt; Os resultados ressaltam que espécies ecologicamente especializadas são mais fáceis de modelar do que espécies bom grandes distribuições</t>
+  </si>
+  <si>
+    <t>&gt; Maxent obteve a melhor performance ao permanecer mais fiel, estável na acurácia e na área total presente ao longo dos diferentes tamanhos de amostras. Obteve a maior acurácia e concordância espacial, ao comparar com o modelos com todas as ocorrências.</t>
+  </si>
+  <si>
+    <t>&gt; Bioclim não mostrou-se capaz de maximizar sua acurácia quando com poucas ocorrências e não performou tão bem quanto os outros métodos em datasets maiores. Os autores sugeriram não usá-lo em datasets com poucas ocorrências.</t>
+  </si>
+  <si>
+    <t>&gt; Domain e GARP performaram de maneira similar, contudo Domain se sobressai, ao passo que em duas medidas (AUC e sucesso de predição) mostraram conflitos na avaliação da performance dos modelos do GARP e Domain se manteve mais consistente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The effect of sample size and species characteristics on performance of different species distribution modeling methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Pilar A. Hernandez, Catherine H. Graham, et al. (2006)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity and Distributions
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Using species distribution models to predict new occurrences for rare plants</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+John N. Williams et al. (2009)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Utilizaram 4 métodos de modelagem (Random Forest, Generalized Linear Models, Artificial Neural Networds e Maxent) para gerar modelos de distribuição de 6 espécies de plantas endêmicas raras dos EUA.</t>
+  </si>
+  <si>
+    <t>&gt; RF, GLM e ANN requerem dados de presença também, como não havia dados do tipo, foram utilizados pseudo-ausências 
+selecionadas aleatoriamente. O único modelo que não requer registros de ausência é o Maxent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; Avaliaram os modelos a partir dos métodos estatísticos AUC do ROC e Kappa. </t>
+  </si>
+  <si>
+    <t>&gt; RESULTADOS: &gt; Random Forest obteve o modelo com os melhores índices de AUC e Kappa, embora Maxent obteve resultados próximos. GLM e ANN também obtiveram bons resultados, mas foram menos restritivos e variaram mais do que RF e Maxent.</t>
+  </si>
+  <si>
+    <t>&gt; Através do exame dos mapas criados e estatísticas de correlação, observaram que RF e Maxent geraram modelos similares tanto em termos de valores do AUC quanto as localidades onde as ocorrências foram preditas.</t>
+  </si>
+  <si>
+    <t>&gt; ANN e GLM não performaram tão bem quanto os outros modelos, o que pode ser um exemplo de performance incosistente com 
+espécies de prevalência baixa.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Effects of sample size on the performance of species distribution models</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+M. S. Wisz et al. (2008)</t>
+    </r>
+  </si>
+  <si>
+    <t>Diversity and Distributions</t>
+  </si>
+  <si>
+    <t>&gt; Avaliaram a predição de 12 algoritmos para 46 espécies de 6 partes do globo e com 3 tamanhos de amostragem (10, 30 e 100).</t>
+  </si>
+  <si>
+    <t>&gt; Utilizaram como medidas estatística dos modelos o AUC do ROC e o índice de correlação de Pearson (COR).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&gt; Os modelos foram treinados com os registros de ocorrência e então avaliados com os de ausência. </t>
+  </si>
+  <si>
+    <t>&gt; RESULTADOS: O modelo que performou melhor ao longo dos tamanhos diferentes de amostras foi o Maxent. O método obteve sensibilidade moderada dos tamanhos de amostras combinado com ótima capacidade de predição. Foi o segundo melhor modelo a performar com 100 e 30 ocorrências e o melhor com 10 ocorrências.</t>
+  </si>
+  <si>
+    <t>&gt; GBM foi o melhor com 30 e 100 ocorrências, significativamente melhor que Maxent com 100 ocorrências.</t>
+  </si>
+  <si>
+    <t>&gt; Com 10 ocorrências, OM-GARP foi o segundo com a melhor performance. Maxent e OM-GARP mostraram-se os com menor sensibilidade (o quão frequentemente o modelo prediz presenças verdadeiras) com amostras pequenas, performando melhor que outros métodos com poucos dados.</t>
+  </si>
+  <si>
+    <t>&gt; O estudo está de acordo com outros, mostrando que a performance dos modelos aumentam, enquanto que a acurácia de predição diminui com o aumento do número de ocorrências.</t>
+  </si>
+  <si>
+    <t>Novel methods improve prediction of species’ distributions from occurrence data
+Jane Elith et al. (2006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; Compararam 16 métodos de modelagem para 226 espécies de 6 regiões do planeta. Foram usados dados de presença para treinar 
+os modelos e de ausência para avaliar as predições. 
+</t>
+  </si>
+  <si>
+    <t>&gt; Para a avaliação dos modelos gerados foram utilizados o AUC do ROC, índice de correlação de Pearson e Kappa</t>
+  </si>
+  <si>
+    <t>&gt; Comparações dos 16 modelos foram criadas resumidas das 50.000 interações Monte Carlo feitas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; RESULTADOS: O grupo de modelos com as melhores performances ao longo de todas as espécies de acordo com as medidas de avaliação foram MARS, BRT, Maxent e GDM respectivamente.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Maximum entropy modelling of species geographic distributions 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Steven J. Phillips, Robert P. Anderson, Robert E. Schapire (2006)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Ecological modelling</t>
+  </si>
+  <si>
+    <t>&gt; Compararam os modelos de distribuição gerados pelo Maxent e GARP de duas espécies (uma de preguiça e outra de roedor, ambas com mais de 80 ocorrências) da América do Sul.</t>
+  </si>
+  <si>
+    <t>&gt; Avaliaram e compararam os modelos com base nos métodos estatísticos AUC do ROC e o teste de “equalized predicted area”.</t>
+  </si>
+  <si>
+    <t>RESULTADOS: &gt; Ambos os algoritmos performaram bem, embora Maxent obteve resultados melhores do que o GARP.</t>
+  </si>
+  <si>
+    <t>&gt; A Área Sob a Curva (AUC) do ROC foi significativamente melhor para os modelos produzidos pelo Maxent em quase todas as partições dos dados (os autores criaram diversos modelos, variando o threshold, mudando as variáveis ambientais etc) para as duas espécies.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; Interpretação estatística: O teste </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">equalized predicted area </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>geralmente indicou melhor performance do Maxent nas predições da espécie de roedor (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M. minutu),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mas não detectou diferenças significativas entre os algoritmos para a espécies de bicho-preguiça (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B. variegatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Interpretação biológica: Ambos algoritmos apresentaram modelos razoáveis acerca da distribuição potencial da espécie de bicho-preguiça, performando muito melhor do que mapas disponíveis de estudos de campo e e compilações digitais para o uso em conservação. Os modelos indicaram corretamente a expansão de ambientes inadequados, como por exemplo em áreas não florestadas do Cerrado brasileiro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; Diferentemente, os algoritmos divergiram na predição da espécie de roedor. Maxent produziu modelos predições impressionantes acerca do alcance conhecido da espécie, segundo os autores. Maxent predice a distribuição da espécies quase que inteiramente na região dos Andes, embora existam ambientes adequados para a espécies, como no Brasil, mas não são possíveis de serem colonizados por causa de barreiras geográficas. Nesse sentido, Maxent produziu modelos mais corretos do que o GARP. GARP superestimou a distribuição para regiões adequadas, porém além das barreiras geográficas. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,8 +587,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +626,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -284,53 +686,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -338,6 +879,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFCC6600"/>
+      <color rgb="FF0099CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -646,11 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F280F5-24EE-4664-8BA0-7ED3FDBE296D}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,115 +1209,463 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="186" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="290.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="301.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:3" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:3" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="47"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="47"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="47"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="30"/>
+    </row>
+    <row r="54" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="47"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="47"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A56" s="48"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="42" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B21"/>
+    <mergeCell ref="B22:B32"/>
+    <mergeCell ref="A22:A32"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="A33:A38"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>